<commit_message>
feat: new pcb version, removed mess
</commit_message>
<xml_diff>
--- a/drn2/BOM.xlsx
+++ b/drn2/BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
   <si>
     <t>Comment</t>
   </si>
@@ -28,25 +28,37 @@
     <t>LCSC Part Number</t>
   </si>
   <si>
-    <t>LSM6</t>
-  </si>
-  <si>
-    <t>ACCGYRO1</t>
-  </si>
-  <si>
-    <t>LGA-12_2x2mm_P0.5mm</t>
-  </si>
-  <si>
-    <t>C94048</t>
-  </si>
-  <si>
-    <t>LSM303</t>
-  </si>
-  <si>
-    <t>ACCMAG1</t>
-  </si>
-  <si>
-    <t>C126671</t>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>C1,C2,C3</t>
+  </si>
+  <si>
+    <t>C_0603_1608Metric_Pad1.08x0.95mm_HandSolder</t>
+  </si>
+  <si>
+    <t>C66501</t>
+  </si>
+  <si>
+    <t>C_Polarized</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>CP_Elec_4x5.4</t>
+  </si>
+  <si>
+    <t>C213487</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C519406</t>
   </si>
   <si>
     <t>LEDG</t>
@@ -91,7 +103,7 @@
     <t>Conn_01x03_Socket</t>
   </si>
   <si>
-    <t>J1,J3,J4,J7,J8,J9,J10,J11,J12,J13,J14,J15,J16</t>
+    <t>J1,J3,J4,J7,J12,J13,J16</t>
   </si>
   <si>
     <t>PinHeader_1x03_P2.54mm_Vertical</t>
@@ -145,18 +157,6 @@
     <t>J4_M4_BEC_IN1</t>
   </si>
   <si>
-    <t>Conn_01x12_Socket</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>JST_XH_B12B-XH-AM_1x12_P2.50mm_Vertical</t>
-  </si>
-  <si>
-    <t>C157941</t>
-  </si>
-  <si>
     <t>Conn_01x08_Socket</t>
   </si>
   <si>
@@ -169,10 +169,16 @@
     <t>C6332201</t>
   </si>
   <si>
+    <t>J14GND1</t>
+  </si>
+  <si>
+    <t>J15VBECOUT1</t>
+  </si>
+  <si>
     <t>130</t>
   </si>
   <si>
-    <t>R1,R2,R3</t>
+    <t>R1,R2,R3,R8,R9,R10,R11</t>
   </si>
   <si>
     <t>R_0603_1608Metric</t>
@@ -188,6 +194,15 @@
   </si>
   <si>
     <t>C23185</t>
+  </si>
+  <si>
+    <t>LSM9DS1</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>LGA-24L_3x3.5mm_P0.43mm</t>
   </si>
 </sst>
 </file>
@@ -519,7 +534,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -564,21 +579,21 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -592,49 +607,49 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -670,100 +685,100 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
         <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -782,30 +797,69 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
         <v>55</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D21" t="s">
         <v>56</v>
       </c>
-      <c r="C20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v4 done, requires FP check
</commit_message>
<xml_diff>
--- a/drn2/BOM.xlsx
+++ b/drn2/BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t>Comment</t>
   </si>
@@ -28,6 +28,18 @@
     <t>LCSC Part Number</t>
   </si>
   <si>
+    <t>Conn_01x03_Socket</t>
+  </si>
+  <si>
+    <t>5V1</t>
+  </si>
+  <si>
+    <t>PinHeader_1x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>C541850</t>
+  </si>
+  <si>
     <t>100nF</t>
   </si>
   <si>
@@ -100,16 +112,40 @@
     <t>C412284</t>
   </si>
   <si>
-    <t>Conn_01x03_Socket</t>
-  </si>
-  <si>
-    <t>J1,J3,J4,J7,J16</t>
-  </si>
-  <si>
-    <t>PinHeader_1x03_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>C49257</t>
+    <t>GND1</t>
+  </si>
+  <si>
+    <t>Conn_01x04_Socket</t>
+  </si>
+  <si>
+    <t>I2C1</t>
+  </si>
+  <si>
+    <t>PinHeader_1x04_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>C2718488</t>
+  </si>
+  <si>
+    <t>LSM9DS1</t>
+  </si>
+  <si>
+    <t>IMU1</t>
+  </si>
+  <si>
+    <t>LGA-24L_3x3.5mm_P0.43mm</t>
+  </si>
+  <si>
+    <t>C2655096</t>
+  </si>
+  <si>
+    <t>J1,J3,J4,J7,J37</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>PinSocket_1x04_P2.54mm_Vertical</t>
   </si>
   <si>
     <t>Conn_01x02_Pin</t>
@@ -148,25 +184,19 @@
     <t>JST_XH_B4B-XH-A_1x04_P2.50mm_Vertical</t>
   </si>
   <si>
-    <t>C161870</t>
-  </si>
-  <si>
-    <t>Conn_01x09_Socket</t>
-  </si>
-  <si>
-    <t>J10</t>
-  </si>
-  <si>
-    <t>PinHeader_1x09_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>C7509520</t>
-  </si>
-  <si>
-    <t>J14GND1</t>
-  </si>
-  <si>
-    <t>J15VBECOUT1</t>
+    <t>C18077835</t>
+  </si>
+  <si>
+    <t>ADS1115IDGS</t>
+  </si>
+  <si>
+    <t>MAN1</t>
+  </si>
+  <si>
+    <t>TSSOP-10_3x3mm_P0.5mm</t>
+  </si>
+  <si>
+    <t>C37593</t>
   </si>
   <si>
     <t>130</t>
@@ -211,7 +241,7 @@
     <t>Raspberry_Pi_2_3</t>
   </si>
   <si>
-    <t>RPI02</t>
+    <t>RPI2</t>
   </si>
   <si>
     <t>Raspberry_Pi_Zero_Socketed_THT_FaceDown_MountingHoles</t>
@@ -220,28 +250,10 @@
     <t>C2977589</t>
   </si>
   <si>
-    <t>LSM9DS1</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>LGA-24L_3x3.5mm_P0.43mm</t>
-  </si>
-  <si>
-    <t>C2655096</t>
-  </si>
-  <si>
-    <t>MCP3004</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>DIP-14_W7.62mm</t>
-  </si>
-  <si>
-    <t>C512186</t>
+    <t>SPI1</t>
+  </si>
+  <si>
+    <t>UART1</t>
   </si>
 </sst>
 </file>
@@ -573,7 +585,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -632,21 +644,21 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -660,49 +672,49 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -710,167 +722,167 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
         <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
         <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
         <v>55</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>56</v>
-      </c>
-      <c r="C20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
         <v>58</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>59</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
       </c>
       <c r="D21" t="s">
         <v>60</v>
@@ -884,21 +896,21 @@
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
         <v>67</v>
@@ -912,24 +924,66 @@
         <v>69</v>
       </c>
       <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
         <v>70</v>
-      </c>
-      <c r="D24" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" t="s">
         <v>73</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
         <v>74</v>
       </c>
-      <c r="D25" t="s">
+      <c r="B26" t="s">
         <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>